<commit_message>
edit excel by Thang
</commit_message>
<xml_diff>
--- a/PhanTich - Thiet Ke - CarPoly/ASM_Excel.xlsx
+++ b/PhanTich - Thiet Ke - CarPoly/ASM_Excel.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai Lieu\KyThuatPhanMem\CarPoly\PhanTich - Thiet Ke - CarPoly\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Nhóm: 7</t>
   </si>
@@ -93,12 +88,36 @@
   </si>
   <si>
     <t>SV3:</t>
+  </si>
+  <si>
+    <t>Vương Thế Minh Thăng</t>
+  </si>
+  <si>
+    <t>PS09070</t>
+  </si>
+  <si>
+    <t>Võ Thành Long</t>
+  </si>
+  <si>
+    <t>Hoàng Hồng Sơn</t>
+  </si>
+  <si>
+    <t>Phạm Lê Huy</t>
+  </si>
+  <si>
+    <t>SV1, SV2</t>
+  </si>
+  <si>
+    <t>SV1</t>
+  </si>
+  <si>
+    <t>SV2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,16 +198,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -196,8 +218,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -206,42 +228,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -386,6 +372,42 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -400,17 +422,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:H23" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:H23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A15:H23"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="STT" dataDxfId="9"/>
-    <tableColumn id="2" name="Tên công việc" dataDxfId="8"/>
-    <tableColumn id="3" name="Thời gian (ngày)" dataDxfId="7"/>
-    <tableColumn id="4" name="Việc trước" dataDxfId="6"/>
-    <tableColumn id="5" name="Ngày bắt đầu" dataDxfId="5"/>
-    <tableColumn id="6" name="Ngày kết thúc" dataDxfId="4"/>
-    <tableColumn id="7" name="Người thực hiện" dataDxfId="3"/>
-    <tableColumn id="8" name="Hoàn thành (%)" dataDxfId="2"/>
+    <tableColumn id="1" name="STT" dataDxfId="7"/>
+    <tableColumn id="2" name="Tên công việc" dataDxfId="6"/>
+    <tableColumn id="3" name="Thời gian (ngày)" dataDxfId="5"/>
+    <tableColumn id="4" name="Việc trước" dataDxfId="4"/>
+    <tableColumn id="5" name="Ngày bắt đầu" dataDxfId="3"/>
+    <tableColumn id="6" name="Ngày kết thúc" dataDxfId="2"/>
+    <tableColumn id="7" name="Người thực hiện" dataDxfId="1"/>
+    <tableColumn id="8" name="Hoàn thành (%)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -671,7 +693,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -681,179 +703,254 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="16" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>1</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>2</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>3</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="C18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>4</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>5</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>6</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>7</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A9:C9"/>

</xml_diff>

<commit_message>
Not thing to commit :)
</commit_message>
<xml_diff>
--- a/PhanTich - Thiet Ke - CarPoly/ASM_Excel.xlsx
+++ b/PhanTich - Thiet Ke - CarPoly/ASM_Excel.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai Lieu\KyThuatPhanMem\CarPoly\PhanTich - Thiet Ke - CarPoly\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
-  <si>
-    <t>Nhóm: 7</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>BẢNG PHÂN CÔNG</t>
   </si>
@@ -112,13 +114,31 @@
   </si>
   <si>
     <t>SV2</t>
+  </si>
+  <si>
+    <t>PS09108</t>
+  </si>
+  <si>
+    <t>Lớp:</t>
+  </si>
+  <si>
+    <t>UD14311</t>
+  </si>
+  <si>
+    <t>Nhóm:</t>
+  </si>
+  <si>
+    <t>SV3</t>
+  </si>
+  <si>
+    <t>SV4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +166,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -198,7 +225,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,14 +239,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -693,7 +729,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,259 +737,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="9.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="6" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="7">
+        <v>27</v>
+      </c>
+      <c r="H16" s="5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="7">
+        <v>27</v>
+      </c>
+      <c r="H17" s="5">
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="7">
+        <v>34</v>
+      </c>
+      <c r="H18" s="5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" s="7">
+        <v>27</v>
+      </c>
+      <c r="H19" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="7">
+        <v>28</v>
+      </c>
+      <c r="H20" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="7">
+        <v>29</v>
+      </c>
+      <c r="H21" s="5">
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A9:C9"/>
+  <mergeCells count="2">
     <mergeCell ref="B4:G6"/>
     <mergeCell ref="B7:G7"/>
   </mergeCells>

</xml_diff>